<commit_message>
Worked on adding pin numbers
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E39754C-1CD9-4E64-AC36-59D80A0542AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D80C99-5441-4635-93EE-4E5B34E809D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Accessory</t>
   </si>
@@ -52,12 +52,6 @@
     <t>Mega</t>
   </si>
   <si>
-    <t>BMP</t>
-  </si>
-  <si>
-    <t>CE</t>
-  </si>
-  <si>
     <t>CS</t>
   </si>
   <si>
@@ -76,7 +70,52 @@
     <t>https://docs.arduino.cc/static/2de2c8ff00fc05065634e3823a9266c4/A000067-pinout.png</t>
   </si>
   <si>
-    <t>…</t>
+    <t>BNO055IMU</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>3vo</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>side1</t>
+  </si>
+  <si>
+    <t>side2</t>
+  </si>
+  <si>
+    <t>SD Adapter</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>NRF24l01 standard</t>
   </si>
 </sst>
 </file>
@@ -121,13 +160,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -136,7 +172,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -453,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,104 +509,161 @@
     <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="L3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -573,7 +672,7 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -638,93 +737,96 @@
       <c r="O27" s="1"/>
     </row>
     <row r="35" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="3"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
     </row>
     <row r="36" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
+      <c r="C36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="D37" s="5"/>
       <c r="E37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-    </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="F37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+    </row>
+    <row r="38" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-    </row>
-    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="F38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+    </row>
+    <row r="39" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
+      <c r="F39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="C1:R1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="F37:R37"/>
     <mergeCell ref="F38:R38"/>
     <mergeCell ref="F39:R39"/>
-    <mergeCell ref="C36:D39"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C1:R1"/>
-    <mergeCell ref="A2:A20"/>
-    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C37:D39"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F37" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>

</xml_diff>

<commit_message>
Update Pins for Mega NRF
Added NRF (standard) pins to the Pins library for Mega 2560, following the Nano
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64495274-A320-4AD7-8FE8-D0BAF39A0F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D03D1C-C359-47F2-8728-B63FE243F663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
+    <workbookView xWindow="-48945" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Accessory</t>
   </si>
@@ -55,9 +55,6 @@
     <t>CS</t>
   </si>
   <si>
-    <t xml:space="preserve">Microcontroller pin numbers are according to </t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>https://docs.arduino.cc/static/6ec5e4c2a6c0e9e46389d4f6dc924073/A000066-pinout.png</t>
   </si>
   <si>
-    <t>https://docs.arduino.cc/static/2de2c8ff00fc05065634e3823a9266c4/A000067-pinout.png</t>
-  </si>
-  <si>
     <t>BNO055IMU</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
     <t>D12 - MISO</t>
   </si>
   <si>
-    <t>D9</t>
-  </si>
-  <si>
     <t>D7</t>
   </si>
   <si>
@@ -155,6 +146,33 @@
   </si>
   <si>
     <t>5V not VIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin numbers are according to </t>
+  </si>
+  <si>
+    <t>NRF24l01</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>https://www.electronicshub.org/wp-content/uploads/2021/01/Arduino-Mega-Pinout.jpg</t>
+  </si>
+  <si>
+    <t>https://lastminuteengineers.com/nrf24l01-arduino-wireless-communication/</t>
+  </si>
+  <si>
+    <t>3V3</t>
+  </si>
+  <si>
+    <t>52 - SCK</t>
+  </si>
+  <si>
+    <t>50 - MISO</t>
+  </si>
+  <si>
+    <t>51 - MOSI</t>
   </si>
 </sst>
 </file>
@@ -210,17 +228,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -537,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,206 +576,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="6"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="4"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="R3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="K4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="N4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="T4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="W4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -875,86 +914,103 @@
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="4"/>
+      <c r="C36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="7"/>
+      <c r="C37" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
+      <c r="F37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
     </row>
     <row r="38" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
+      <c r="F38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
     </row>
     <row r="39" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
+      <c r="F39" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+    </row>
+    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="F37:R37"/>
-    <mergeCell ref="F38:R38"/>
-    <mergeCell ref="F39:R39"/>
-    <mergeCell ref="C37:D39"/>
-    <mergeCell ref="C36:D36"/>
+  <mergeCells count="13">
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="C1:R1"/>
     <mergeCell ref="A2:A6"/>
@@ -962,13 +1018,20 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
+    <mergeCell ref="F37:R37"/>
+    <mergeCell ref="F38:R38"/>
+    <mergeCell ref="F39:R39"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D40"/>
+    <mergeCell ref="F40:R40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F37" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>
     <hyperlink ref="F38" r:id="rId2" xr:uid="{5050C1D4-A2B3-49B0-A31A-26368B5FB3AE}"/>
     <hyperlink ref="F39" r:id="rId3" xr:uid="{22D30853-0A8C-4606-A419-D79377A024AE}"/>
+    <hyperlink ref="F40" r:id="rId4" xr:uid="{71C3A2A6-029A-49E1-8624-C845751B4B71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added second nano pinout diagram to Pins
Added second nano pinout to Pins that includes the default pin numbers (not D)
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D03D1C-C359-47F2-8728-B63FE243F663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686DE8AF-2AD0-454E-A597-F7FD59549799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48945" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>https://i2.wp.com/www.teachmemicro.com/wp-content/uploads/2019/06/Arduino-Nano-pinout.jpg?fit=1500%2C1500&amp;ssl=1</t>
-  </si>
-  <si>
     <t>https://docs.arduino.cc/static/6ec5e4c2a6c0e9e46389d4f6dc924073/A000066-pinout.png</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>51 - MOSI</t>
+  </si>
+  <si>
+    <t>https://i2.wp.com/www.teachmemicro.com/wp-content/uploads/2019/06/Arduino-Nano-pinout.jpg?fit=1500%2C1500&amp;ssl=1 + https://www.makerguides.com/wp-content/uploads/2020/10/arduino-nano-every-pinout.png</t>
   </si>
 </sst>
 </file>
@@ -228,17 +228,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -555,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,227 +576,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="4"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="6"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="S3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="V3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="P4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="V4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T6" s="2" t="s">
+      <c r="U6" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -909,92 +909,116 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
+    <row r="36" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="5"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="7"/>
       <c r="E37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-    </row>
-    <row r="38" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="F37" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="6"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="6"/>
+    </row>
+    <row r="38" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
       <c r="E38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-    </row>
-    <row r="39" spans="3:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="F38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
+      <c r="U38" s="6"/>
+      <c r="V38" s="6"/>
+      <c r="W38" s="6"/>
+      <c r="X38" s="6"/>
+      <c r="Y38" s="6"/>
+      <c r="Z38" s="6"/>
+    </row>
+    <row r="39" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
       <c r="E39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
+      <c r="U39" s="6"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="6"/>
+      <c r="Z39" s="6"/>
+    </row>
+    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-    </row>
-    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -1008,9 +1032,23 @@
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
+      <c r="U40" s="6"/>
+      <c r="V40" s="6"/>
+      <c r="W40" s="6"/>
+      <c r="X40" s="6"/>
+      <c r="Y40" s="6"/>
+      <c r="Z40" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D40"/>
+    <mergeCell ref="F37:Z37"/>
+    <mergeCell ref="F38:Z38"/>
+    <mergeCell ref="F39:Z39"/>
+    <mergeCell ref="F40:Z40"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="C1:R1"/>
     <mergeCell ref="A2:A6"/>
@@ -1018,15 +1056,9 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
-    <mergeCell ref="F37:R37"/>
-    <mergeCell ref="F38:R38"/>
-    <mergeCell ref="F39:R39"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D40"/>
-    <mergeCell ref="F40:R40"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F37" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>
+    <hyperlink ref="F37" r:id="rId1" display="https://i2.wp.com/www.teachmemicro.com/wp-content/uploads/2019/06/Arduino-Nano-pinout.jpg?fit=1500%2C1500&amp;ssl=1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>
     <hyperlink ref="F38" r:id="rId2" xr:uid="{5050C1D4-A2B3-49B0-A31A-26368B5FB3AE}"/>
     <hyperlink ref="F39" r:id="rId3" xr:uid="{22D30853-0A8C-4606-A419-D79377A024AE}"/>
     <hyperlink ref="F40" r:id="rId4" xr:uid="{71C3A2A6-029A-49E1-8624-C845751B4B71}"/>

</xml_diff>

<commit_message>
Added code to realign with tutorial for NRF
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686DE8AF-2AD0-454E-A597-F7FD59549799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D633E5D-86E8-4CEE-B5DB-CA74F7F1B8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
+    <workbookView xWindow="-51510" yWindow="5040" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Accessory</t>
   </si>
@@ -172,7 +172,16 @@
     <t>51 - MOSI</t>
   </si>
   <si>
-    <t>https://i2.wp.com/www.teachmemicro.com/wp-content/uploads/2019/06/Arduino-Nano-pinout.jpg?fit=1500%2C1500&amp;ssl=1 + https://www.makerguides.com/wp-content/uploads/2020/10/arduino-nano-every-pinout.png</t>
+    <t>https://i2.wp.com/www.teachmemicro.com/wp-content/uploads/2019/06/Arduino-Nano-pinout.jpg?fit=1500%2C1500&amp;ssl=1</t>
+  </si>
+  <si>
+    <t>https://www.makerguides.com/wp-content/uploads/2020/10/arduino-nano-every-pinout.png</t>
+  </si>
+  <si>
+    <t>Nano2</t>
+  </si>
+  <si>
+    <t>Nano1</t>
   </si>
 </sst>
 </file>
@@ -217,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -232,13 +241,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -555,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
-  <dimension ref="A1:Z40"/>
+  <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,63 +588,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4" t="s">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="4"/>
+      <c r="W2" s="5"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="8"/>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
@@ -698,7 +710,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -767,13 +779,13 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -914,141 +926,165 @@
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="7" t="s">
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" s="6" t="s">
+      <c r="D37" s="6"/>
+      <c r="E37" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
+    </row>
+    <row r="38" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
-      <c r="U37" s="6"/>
-      <c r="V37" s="6"/>
-      <c r="W37" s="6"/>
-      <c r="X37" s="6"/>
-      <c r="Y37" s="6"/>
-      <c r="Z37" s="6"/>
-    </row>
-    <row r="38" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="2" t="s">
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+    </row>
+    <row r="39" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="6"/>
-      <c r="Y38" s="6"/>
-      <c r="Z38" s="6"/>
-    </row>
-    <row r="39" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="2" t="s">
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7"/>
+    </row>
+    <row r="40" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F40" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="6"/>
-      <c r="U39" s="6"/>
-      <c r="V39" s="6"/>
-      <c r="W39" s="6"/>
-      <c r="X39" s="6"/>
-      <c r="Y39" s="6"/>
-      <c r="Z39" s="6"/>
-    </row>
-    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="2" t="s">
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="7"/>
+    </row>
+    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F41" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="6"/>
-      <c r="U40" s="6"/>
-      <c r="V40" s="6"/>
-      <c r="W40" s="6"/>
-      <c r="X40" s="6"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D40"/>
-    <mergeCell ref="F37:Z37"/>
-    <mergeCell ref="F38:Z38"/>
-    <mergeCell ref="F39:Z39"/>
-    <mergeCell ref="F40:Z40"/>
+  <mergeCells count="14">
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="C1:R1"/>
     <mergeCell ref="A2:A6"/>
@@ -1056,14 +1092,22 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F38:Z38"/>
+    <mergeCell ref="F39:Z39"/>
+    <mergeCell ref="F40:Z40"/>
+    <mergeCell ref="F41:Z41"/>
+    <mergeCell ref="F37:Z37"/>
+    <mergeCell ref="C37:D41"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F37" r:id="rId1" display="https://i2.wp.com/www.teachmemicro.com/wp-content/uploads/2019/06/Arduino-Nano-pinout.jpg?fit=1500%2C1500&amp;ssl=1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>
-    <hyperlink ref="F38" r:id="rId2" xr:uid="{5050C1D4-A2B3-49B0-A31A-26368B5FB3AE}"/>
-    <hyperlink ref="F39" r:id="rId3" xr:uid="{22D30853-0A8C-4606-A419-D79377A024AE}"/>
-    <hyperlink ref="F40" r:id="rId4" xr:uid="{71C3A2A6-029A-49E1-8624-C845751B4B71}"/>
+    <hyperlink ref="F38" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>
+    <hyperlink ref="F39" r:id="rId2" xr:uid="{5050C1D4-A2B3-49B0-A31A-26368B5FB3AE}"/>
+    <hyperlink ref="F40" r:id="rId3" xr:uid="{22D30853-0A8C-4606-A419-D79377A024AE}"/>
+    <hyperlink ref="F41" r:id="rId4" xr:uid="{71C3A2A6-029A-49E1-8624-C845751B4B71}"/>
+    <hyperlink ref="F37" r:id="rId5" xr:uid="{231EDB6C-6681-400B-9EFF-958059104670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Pins for NRF test success
Updated the Pins microcontroller reference docs to reflect the newest hardware. Update the Pins to reflect successful NRF test and resolving of Issue #2
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D633E5D-86E8-4CEE-B5DB-CA74F7F1B8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E14448-182E-4C45-9F4F-132EC55B2B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51510" yWindow="5040" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
+    <workbookView xWindow="-53400" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Accessory</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Key</t>
   </si>
   <si>
-    <t>https://docs.arduino.cc/static/6ec5e4c2a6c0e9e46389d4f6dc924073/A000066-pinout.png</t>
-  </si>
-  <si>
     <t>BNO055IMU</t>
   </si>
   <si>
@@ -154,12 +151,6 @@
     <t>D8</t>
   </si>
   <si>
-    <t>https://www.electronicshub.org/wp-content/uploads/2021/01/Arduino-Mega-Pinout.jpg</t>
-  </si>
-  <si>
-    <t>https://lastminuteengineers.com/nrf24l01-arduino-wireless-communication/</t>
-  </si>
-  <si>
     <t>3V3</t>
   </si>
   <si>
@@ -172,16 +163,16 @@
     <t>51 - MOSI</t>
   </si>
   <si>
-    <t>https://i2.wp.com/www.teachmemicro.com/wp-content/uploads/2019/06/Arduino-Nano-pinout.jpg?fit=1500%2C1500&amp;ssl=1</t>
-  </si>
-  <si>
-    <t>https://www.makerguides.com/wp-content/uploads/2020/10/arduino-nano-every-pinout.png</t>
-  </si>
-  <si>
-    <t>Nano2</t>
-  </si>
-  <si>
-    <t>Nano1</t>
+    <t>https://howtomechatronics.com/tutorials/arduino/arduino-wireless-communication-nrf24l01-tutorial/</t>
+  </si>
+  <si>
+    <t>https://content.arduino.cc/assets/Pinout-NANO_latest.pdf?_gl=1*xob608*_ga*NzQ0NDIyMTcuMTY0MjkwMDQ5Nw..*_ga_NEXN8H46L5*MTY1NTU5OTgyNy4yMS4xLjE2NTU1OTk5NjkuNDk.</t>
+  </si>
+  <si>
+    <t>https://content.arduino.cc/assets/Pinout-Mega2560rev3_latest.pdf?_gl=1*xf3c7r*_ga*NzQ0NDIyMTcuMTY0MjkwMDQ5Nw..*_ga_NEXN8H46L5*MTY1NTYwNDAyNS4yMi4xLjE2NTU2MDQyMDguNTM.</t>
+  </si>
+  <si>
+    <t>https://content.arduino.cc/assets/Pinout-UNOrev3_latest.pdf?_gl=1*1ehfkp*_ga*NzQ0NDIyMTcuMTY0MjkwMDQ5Nw..*_ga_NEXN8H46L5*MTY1NTYwNDAyNS4yMi4xLjE2NTU2MDQyMzcuMjQ.</t>
   </si>
 </sst>
 </file>
@@ -226,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -244,13 +235,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -569,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,21 +602,21 @@
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -630,7 +624,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -639,176 +633,176 @@
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W2" s="5"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="6"/>
       <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="S3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="V3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="O4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="V4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="T6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -932,45 +926,40 @@
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
-      <c r="V37" s="5"/>
-      <c r="W37" s="5"/>
-      <c r="X37" s="5"/>
-      <c r="Y37" s="5"/>
-      <c r="Z37" s="5"/>
+      <c r="C37" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
       <c r="E38" s="2" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -994,13 +983,13 @@
       <c r="Z38" s="7"/>
     </row>
     <row r="39" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
       <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -1024,13 +1013,13 @@
       <c r="Z39" s="7"/>
     </row>
     <row r="40" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
       <c r="E40" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
@@ -1054,13 +1043,13 @@
       <c r="Z40" s="7"/>
     </row>
     <row r="41" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
       <c r="E41" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -1084,7 +1073,13 @@
       <c r="Z41" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F38:Z38"/>
+    <mergeCell ref="F39:Z39"/>
+    <mergeCell ref="F40:Z40"/>
+    <mergeCell ref="F41:Z41"/>
+    <mergeCell ref="C37:D41"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="C1:R1"/>
     <mergeCell ref="A2:A6"/>
@@ -1092,22 +1087,14 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="F38:Z38"/>
-    <mergeCell ref="F39:Z39"/>
-    <mergeCell ref="F40:Z40"/>
-    <mergeCell ref="F41:Z41"/>
-    <mergeCell ref="F37:Z37"/>
-    <mergeCell ref="C37:D41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F38" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>
     <hyperlink ref="F39" r:id="rId2" xr:uid="{5050C1D4-A2B3-49B0-A31A-26368B5FB3AE}"/>
     <hyperlink ref="F40" r:id="rId3" xr:uid="{22D30853-0A8C-4606-A419-D79377A024AE}"/>
     <hyperlink ref="F41" r:id="rId4" xr:uid="{71C3A2A6-029A-49E1-8624-C845751B4B71}"/>
-    <hyperlink ref="F37" r:id="rId5" xr:uid="{231EDB6C-6681-400B-9EFF-958059104670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Pins and SKIP
Add Key to understand new naming system like CIPO and COPI. Success of NRF test Fixes #2
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E14448-182E-4C45-9F4F-132EC55B2B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E02D28F-6D31-4561-B383-12E3427D6F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-53400" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>Accessory</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>https://content.arduino.cc/assets/Pinout-UNOrev3_latest.pdf?_gl=1*1ehfkp*_ga*NzQ0NDIyMTcuMTY0MjkwMDQ5Nw..*_ga_NEXN8H46L5*MTY1NTYwNDAyNS4yMi4xLjE2NTU2MDQyMzcuMjQ.</t>
+  </si>
+  <si>
+    <t>MOSI = COPI, MISO = CIPO, CS = SS</t>
   </si>
 </sst>
 </file>
@@ -231,11 +234,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,8 +246,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -563,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,63 +585,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5" t="s">
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="W2" s="5"/>
+      <c r="W2" s="6"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -704,7 +707,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -773,13 +776,13 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -920,17 +923,23 @@
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D37" s="8"/>
-      <c r="F37" s="9"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -1073,13 +1082,7 @@
       <c r="Z41" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="F38:Z38"/>
-    <mergeCell ref="F39:Z39"/>
-    <mergeCell ref="F40:Z40"/>
-    <mergeCell ref="F41:Z41"/>
-    <mergeCell ref="C37:D41"/>
+  <mergeCells count="14">
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="C1:R1"/>
     <mergeCell ref="A2:A6"/>
@@ -1087,6 +1090,13 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F38:Z38"/>
+    <mergeCell ref="F39:Z39"/>
+    <mergeCell ref="F40:Z40"/>
+    <mergeCell ref="F41:Z41"/>
+    <mergeCell ref="C37:D41"/>
+    <mergeCell ref="E36:H36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F38" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>

</xml_diff>